<commit_message>
Interface del sistema agregada pero incompleta
</commit_message>
<xml_diff>
--- a/Graphs/Modelo R.xlsx
+++ b/Graphs/Modelo R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\My Homeworks\acceso por carpetas\De carrera\9 semestre\arq de sistemas\primera vez\tareas\conserjeria\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E69B753-666F-418D-B950-5BC7AF86F781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD33A6FA-F314-4C82-9968-29C85E73B13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,12 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +453,7 @@
   <dimension ref="B4:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,13 +505,13 @@
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -553,7 +552,7 @@
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="3" t="s">

</xml_diff>

<commit_message>
Se añadieron los pagos y se ha hecho una pequeña modificacion en la base de datos.
</commit_message>
<xml_diff>
--- a/Graphs/Modelo R.xlsx
+++ b/Graphs/Modelo R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\My Homeworks\acceso por carpetas\De carrera\9 semestre\arq de sistemas\primera vez\tareas\conserjeria\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD33A6FA-F314-4C82-9968-29C85E73B13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022D2F2B-90A9-4900-BB9F-3A642291A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Depto</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>IDDueño</t>
+  </si>
+  <si>
+    <t>IDDepto</t>
   </si>
 </sst>
 </file>
@@ -453,17 +456,17 @@
   <dimension ref="B4:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -476,16 +479,13 @@
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -496,12 +496,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -515,7 +515,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -557,6 +557,9 @@
       </c>
       <c r="D21" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clases modificadas y corregidas
</commit_message>
<xml_diff>
--- a/Graphs/Modelo R.xlsx
+++ b/Graphs/Modelo R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\My Homeworks\acceso por carpetas\De carrera\9 semestre\arq de sistemas\primera vez\tareas\conserjeria\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022D2F2B-90A9-4900-BB9F-3A642291A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936BB11C-AEA3-4E6B-AB66-1703394CBDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Depto</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>IDEdificio</t>
-  </si>
-  <si>
-    <t>tipo</t>
   </si>
   <si>
     <t>FechaDeGastos</t>
@@ -453,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:H21"/>
+  <dimension ref="B4:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +509,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
@@ -520,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
@@ -539,27 +536,24 @@
       <c r="G17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>